<commit_message>
A bunch of changes and new tests for harvesting ContentArchives; Bugfix for NameLink
</commit_message>
<xml_diff>
--- a/tests/fixtures/files/new_schema_spreadsheet.xlsx
+++ b/tests/fixtures/files/new_schema_spreadsheet.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="21721"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="20480" tabRatio="704"/>
+    <workbookView xWindow="-30660" yWindow="11000" windowWidth="33600" windowHeight="20480" tabRatio="704" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="media" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="411" uniqueCount="375">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="414" uniqueCount="378">
   <si>
     <t>Not Applicable</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -216,10 +216,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>http://eol.org/schema/media/agentID</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>http://eol.org/schema/media/referenceID</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -271,10 +267,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>http://eol.org/schema/media/referenceID</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>http://rs.tdwg.org/dwc/terms/taxonRank</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -566,10 +558,6 @@
     <t>http://purl.org/ontology/bibo/edition</t>
   </si>
   <si>
-    <t>http://eol.org/schema/reference/full_reference</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>http://purl.org/ontology/bibo/doi</t>
   </si>
   <si>
@@ -1046,21 +1034,12 @@
     <t>PublicationType</t>
   </si>
   <si>
-    <t>book, journal, journal article, webpage, …</t>
-  </si>
-  <si>
-    <t>eol#publication_type</t>
-  </si>
-  <si>
     <t>PrimaryTitle</t>
   </si>
   <si>
     <t>SecondaryTitle</t>
   </si>
   <si>
-    <t>eol#primary_title</t>
-  </si>
-  <si>
     <t>(thesaurus)</t>
   </si>
   <si>
@@ -1235,9 +1214,6 @@
     <t>An organization this person is affiliated with.</t>
   </si>
   <si>
-    <t>eol#organization</t>
-  </si>
-  <si>
     <t>A logo representing some thing.</t>
   </si>
   <si>
@@ -1283,9 +1259,6 @@
     <t>http://purl.org/dc/dcmitype</t>
   </si>
   <si>
-    <t>eol#role</t>
-  </si>
-  <si>
     <t>(comment)</t>
   </si>
   <si>
@@ -1296,6 +1269,39 @@
   </si>
   <si>
     <t>An entity primarily responsible for making the resource. Creators of text will be considered authors; creators of photographs will be considered photographers, etc.</t>
+  </si>
+  <si>
+    <t>(examples)</t>
+  </si>
+  <si>
+    <t>Map</t>
+  </si>
+  <si>
+    <t>http://purl.org/dc/terms/type/StillImage</t>
+  </si>
+  <si>
+    <t>book, journal, journal article, webpage, etc</t>
+  </si>
+  <si>
+    <t>http://eol.org/schema/reference/referenceID</t>
+  </si>
+  <si>
+    <t>http://eol.org/schema/agent/agentID</t>
+  </si>
+  <si>
+    <t>http://eol.org/schema/reference/fullReference</t>
+  </si>
+  <si>
+    <t>http://eol.org/schema/reference/primaryTitle</t>
+  </si>
+  <si>
+    <t>http://eol.org/schema/reference/publicationType</t>
+  </si>
+  <si>
+    <t>http://eol.org/schema/agent/agentRole</t>
+  </si>
+  <si>
+    <t>http://eol.org/schema/agent/organization</t>
   </si>
 </sst>
 </file>
@@ -1373,7 +1379,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -1473,23 +1479,21 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="hair">
         <color auto="1"/>
       </left>
       <right style="hair">
         <color auto="1"/>
       </right>
-      <top style="hair">
-        <color auto="1"/>
-      </top>
-      <bottom style="medium">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
       <top/>
       <bottom style="medium">
         <color auto="1"/>
@@ -1501,9 +1505,7 @@
       <right style="hair">
         <color auto="1"/>
       </right>
-      <top style="hair">
-        <color auto="1"/>
-      </top>
+      <top/>
       <bottom style="medium">
         <color auto="1"/>
       </bottom>
@@ -1514,16 +1516,23 @@
         <color auto="1"/>
       </left>
       <right/>
-      <top style="hair">
-        <color auto="1"/>
-      </top>
+      <top/>
       <bottom style="medium">
         <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="hair">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="78">
+  <cellStyleXfs count="100">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1602,8 +1611,30 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1632,43 +1663,7 @@
     <xf numFmtId="0" fontId="2" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="6" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="7" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -1710,8 +1705,47 @@
     <xf numFmtId="49" fontId="0" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="6" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="7" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="78">
+  <cellStyles count="100">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1753,6 +1787,17 @@
     <cellStyle name="Followed Hyperlink" xfId="73" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="75" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="77" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="79" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="81" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="83" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="85" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="87" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="89" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="91" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="93" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="95" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="97" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="99" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1789,6 +1834,17 @@
     <cellStyle name="Hyperlink" xfId="72" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="74" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="76" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="78" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="80" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="82" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="84" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="86" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="88" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="90" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="92" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="94" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="96" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="98" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2116,11 +2172,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AJ9"/>
+  <dimension ref="A1:AJ10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="8" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="9" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="T2" sqref="T2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
@@ -2129,7 +2185,7 @@
     <col min="2" max="2" width="14.85546875" style="12" customWidth="1"/>
     <col min="3" max="3" width="21.5703125" style="24" customWidth="1"/>
     <col min="4" max="4" width="18.7109375" style="24" customWidth="1"/>
-    <col min="5" max="5" width="16.85546875" style="4" customWidth="1"/>
+    <col min="5" max="5" width="34.7109375" style="4" customWidth="1"/>
     <col min="6" max="6" width="26.140625" style="1" customWidth="1"/>
     <col min="7" max="7" width="21.42578125" style="8" customWidth="1"/>
     <col min="8" max="8" width="21.28515625" style="10" customWidth="1"/>
@@ -2163,222 +2219,222 @@
   <sheetData>
     <row r="1" spans="1:36" s="21" customFormat="1" ht="24" customHeight="1" thickBot="1">
       <c r="A1" s="21" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="B1" s="21" t="s">
+        <v>134</v>
+      </c>
+      <c r="C1" s="22" t="s">
+        <v>135</v>
+      </c>
+      <c r="D1" s="22" t="s">
         <v>136</v>
       </c>
-      <c r="C1" s="22" t="s">
+      <c r="E1" s="21" t="s">
         <v>137</v>
       </c>
-      <c r="D1" s="22" t="s">
+      <c r="F1" s="21" t="s">
         <v>138</v>
       </c>
-      <c r="E1" s="21" t="s">
+      <c r="G1" s="21" t="s">
         <v>139</v>
       </c>
-      <c r="F1" s="21" t="s">
+      <c r="H1" s="21" t="s">
         <v>140</v>
       </c>
-      <c r="G1" s="21" t="s">
+      <c r="I1" s="21" t="s">
         <v>141</v>
       </c>
-      <c r="H1" s="21" t="s">
-        <v>142</v>
-      </c>
-      <c r="I1" s="21" t="s">
-        <v>143</v>
-      </c>
       <c r="J1" s="21" t="s">
+        <v>159</v>
+      </c>
+      <c r="K1" s="21" t="s">
+        <v>160</v>
+      </c>
+      <c r="L1" s="21" t="s">
+        <v>210</v>
+      </c>
+      <c r="M1" s="21" t="s">
+        <v>161</v>
+      </c>
+      <c r="N1" s="21" t="s">
+        <v>236</v>
+      </c>
+      <c r="O1" s="21" t="s">
         <v>162</v>
       </c>
-      <c r="K1" s="21" t="s">
+      <c r="P1" s="21" t="s">
         <v>163</v>
       </c>
-      <c r="L1" s="21" t="s">
-        <v>213</v>
-      </c>
-      <c r="M1" s="21" t="s">
+      <c r="Q1" s="21" t="s">
         <v>164</v>
       </c>
-      <c r="N1" s="21" t="s">
-        <v>239</v>
-      </c>
-      <c r="O1" s="21" t="s">
+      <c r="R1" s="21" t="s">
         <v>165</v>
       </c>
-      <c r="P1" s="21" t="s">
+      <c r="S1" s="21" t="s">
         <v>166</v>
       </c>
-      <c r="Q1" s="21" t="s">
+      <c r="T1" s="21" t="s">
         <v>167</v>
       </c>
-      <c r="R1" s="21" t="s">
+      <c r="U1" s="21" t="s">
         <v>168</v>
       </c>
-      <c r="S1" s="21" t="s">
+      <c r="V1" s="21" t="s">
         <v>169</v>
       </c>
-      <c r="T1" s="21" t="s">
+      <c r="W1" s="21" t="s">
         <v>170</v>
       </c>
-      <c r="U1" s="21" t="s">
+      <c r="X1" s="21" t="s">
         <v>171</v>
       </c>
-      <c r="V1" s="21" t="s">
+      <c r="Y1" s="21" t="s">
         <v>172</v>
       </c>
-      <c r="W1" s="21" t="s">
+      <c r="Z1" s="21" t="s">
         <v>173</v>
-      </c>
-      <c r="X1" s="21" t="s">
-        <v>174</v>
-      </c>
-      <c r="Y1" s="21" t="s">
-        <v>175</v>
-      </c>
-      <c r="Z1" s="21" t="s">
-        <v>176</v>
       </c>
       <c r="AA1" s="21" t="s">
         <v>6</v>
       </c>
       <c r="AB1" s="25" t="s">
+        <v>174</v>
+      </c>
+      <c r="AC1" s="25" t="s">
+        <v>175</v>
+      </c>
+      <c r="AD1" s="25" t="s">
+        <v>176</v>
+      </c>
+      <c r="AE1" s="21" t="s">
         <v>177</v>
       </c>
-      <c r="AC1" s="25" t="s">
+      <c r="AF1" s="21" t="s">
+        <v>285</v>
+      </c>
+      <c r="AG1" s="21" t="s">
         <v>178</v>
       </c>
-      <c r="AD1" s="25" t="s">
+      <c r="AH1" s="21" t="s">
         <v>179</v>
       </c>
-      <c r="AE1" s="21" t="s">
+      <c r="AI1" s="21" t="s">
         <v>180</v>
       </c>
-      <c r="AF1" s="21" t="s">
-        <v>288</v>
-      </c>
-      <c r="AG1" s="21" t="s">
-        <v>181</v>
-      </c>
-      <c r="AH1" s="21" t="s">
-        <v>182</v>
-      </c>
-      <c r="AI1" s="21" t="s">
-        <v>183</v>
-      </c>
       <c r="AJ1" s="21" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
     </row>
     <row r="2" spans="1:36" ht="14" thickTop="1">
       <c r="A2" s="14" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B2" s="15" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="C2" s="23" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="D2" s="23" t="s">
         <v>38</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="F2" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>214</v>
+      </c>
+      <c r="H2" s="17" t="s">
+        <v>215</v>
+      </c>
+      <c r="I2" s="17" t="s">
         <v>216</v>
       </c>
-      <c r="G2" s="7" t="s">
+      <c r="J2" s="18" t="s">
         <v>217</v>
       </c>
-      <c r="H2" s="17" t="s">
-        <v>218</v>
-      </c>
-      <c r="I2" s="17" t="s">
-        <v>219</v>
-      </c>
-      <c r="J2" s="18" t="s">
-        <v>220</v>
-      </c>
       <c r="K2" s="14" t="s">
+        <v>113</v>
+      </c>
+      <c r="L2" s="14" t="s">
+        <v>114</v>
+      </c>
+      <c r="M2" s="19" t="s">
         <v>115</v>
       </c>
-      <c r="L2" s="14" t="s">
+      <c r="N2" s="19" t="s">
+        <v>237</v>
+      </c>
+      <c r="O2" s="16" t="s">
         <v>116</v>
       </c>
-      <c r="M2" s="19" t="s">
+      <c r="P2" s="16" t="s">
         <v>117</v>
       </c>
-      <c r="N2" s="19" t="s">
-        <v>240</v>
-      </c>
-      <c r="O2" s="16" t="s">
+      <c r="Q2" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="P2" s="16" t="s">
+      <c r="R2" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="Q2" s="2" t="s">
+      <c r="S2" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="R2" s="2" t="s">
+      <c r="T2" s="17" t="s">
         <v>121</v>
       </c>
-      <c r="S2" s="2" t="s">
+      <c r="U2" s="17" t="s">
         <v>122</v>
       </c>
-      <c r="T2" s="17" t="s">
+      <c r="V2" s="17" t="s">
         <v>123</v>
       </c>
-      <c r="U2" s="17" t="s">
+      <c r="W2" s="17" t="s">
         <v>124</v>
       </c>
-      <c r="V2" s="17" t="s">
-        <v>125</v>
-      </c>
-      <c r="W2" s="17" t="s">
-        <v>126</v>
-      </c>
       <c r="X2" s="17" t="s">
+        <v>127</v>
+      </c>
+      <c r="Y2" s="17" t="s">
+        <v>128</v>
+      </c>
+      <c r="Z2" s="17" t="s">
         <v>129</v>
       </c>
-      <c r="Y2" s="17" t="s">
+      <c r="AA2" t="s">
+        <v>372</v>
+      </c>
+      <c r="AB2" s="26" t="s">
         <v>130</v>
       </c>
-      <c r="Z2" s="17" t="s">
+      <c r="AC2" s="26" t="s">
         <v>131</v>
       </c>
-      <c r="AA2" t="s">
-        <v>46</v>
-      </c>
-      <c r="AB2" s="26" t="s">
+      <c r="AD2" s="26" t="s">
         <v>132</v>
       </c>
-      <c r="AC2" s="26" t="s">
-        <v>133</v>
-      </c>
-      <c r="AD2" s="26" t="s">
-        <v>134</v>
-      </c>
       <c r="AE2" s="16" t="s">
+        <v>47</v>
+      </c>
+      <c r="AF2" s="16" t="s">
+        <v>357</v>
+      </c>
+      <c r="AG2" s="16" t="s">
         <v>48</v>
       </c>
-      <c r="AF2" s="16" t="s">
-        <v>364</v>
-      </c>
-      <c r="AG2" s="16" t="s">
+      <c r="AH2" s="16" t="s">
         <v>49</v>
       </c>
-      <c r="AH2" s="16" t="s">
+      <c r="AI2" s="20" t="s">
         <v>50</v>
       </c>
-      <c r="AI2" s="20" t="s">
-        <v>51</v>
-      </c>
       <c r="AJ2" s="2" t="s">
-        <v>61</v>
+        <v>371</v>
       </c>
     </row>
     <row r="3" spans="1:36">
@@ -2386,10 +2442,10 @@
         <v>39</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="T3" s="10" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="4" spans="1:36">
@@ -2397,168 +2453,168 @@
         <v>40</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="AA4" s="10" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="AJ4" s="1" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
     </row>
     <row r="5" spans="1:36">
       <c r="A5" s="6" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="6" spans="1:36">
       <c r="A6" s="6" t="s">
-        <v>296</v>
+        <v>290</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>369</v>
+        <v>362</v>
       </c>
       <c r="Q6" s="1" t="s">
-        <v>368</v>
-      </c>
-    </row>
-    <row r="7" spans="1:36" s="41" customFormat="1" ht="169">
-      <c r="A7" s="42" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="7" spans="1:36" s="29" customFormat="1" ht="169">
+      <c r="A7" s="30" t="s">
+        <v>218</v>
+      </c>
+      <c r="B7" s="31" t="s">
+        <v>219</v>
+      </c>
+      <c r="C7" s="32" t="s">
+        <v>220</v>
+      </c>
+      <c r="D7" s="32" t="s">
         <v>221</v>
       </c>
-      <c r="B7" s="43" t="s">
+      <c r="E7" s="33" t="s">
         <v>222</v>
       </c>
-      <c r="C7" s="44" t="s">
+      <c r="F7" s="34" t="s">
+        <v>355</v>
+      </c>
+      <c r="G7" s="35" t="s">
         <v>223</v>
       </c>
-      <c r="D7" s="44" t="s">
+      <c r="H7" s="36" t="s">
         <v>224</v>
       </c>
-      <c r="E7" s="45" t="s">
+      <c r="I7" s="36" t="s">
         <v>225</v>
       </c>
-      <c r="F7" s="46" t="s">
-        <v>362</v>
-      </c>
-      <c r="G7" s="47" t="s">
+      <c r="J7" s="37" t="s">
         <v>226</v>
       </c>
-      <c r="H7" s="48" t="s">
+      <c r="K7" s="30" t="s">
         <v>227</v>
       </c>
-      <c r="I7" s="48" t="s">
+      <c r="L7" s="30" t="s">
+        <v>229</v>
+      </c>
+      <c r="M7" s="38" t="s">
         <v>228</v>
       </c>
-      <c r="J7" s="49" t="s">
-        <v>229</v>
-      </c>
-      <c r="K7" s="42" t="s">
+      <c r="N7" s="38" t="s">
+        <v>238</v>
+      </c>
+      <c r="O7" s="39" t="s">
+        <v>353</v>
+      </c>
+      <c r="P7" s="39" t="s">
         <v>230</v>
       </c>
-      <c r="L7" s="42" t="s">
+      <c r="Q7" s="34" t="s">
+        <v>329</v>
+      </c>
+      <c r="R7" s="34" t="s">
+        <v>241</v>
+      </c>
+      <c r="S7" s="34" t="s">
+        <v>231</v>
+      </c>
+      <c r="T7" s="36" t="s">
         <v>232</v>
       </c>
-      <c r="M7" s="50" t="s">
-        <v>231</v>
-      </c>
-      <c r="N7" s="50" t="s">
-        <v>241</v>
-      </c>
-      <c r="O7" s="51" t="s">
+      <c r="U7" s="36" t="s">
+        <v>352</v>
+      </c>
+      <c r="V7" s="36" t="s">
+        <v>239</v>
+      </c>
+      <c r="W7" s="36" t="s">
+        <v>240</v>
+      </c>
+      <c r="X7" s="36" t="s">
+        <v>330</v>
+      </c>
+      <c r="Y7" s="36" t="s">
+        <v>331</v>
+      </c>
+      <c r="Z7" s="36" t="s">
+        <v>366</v>
+      </c>
+      <c r="AA7" s="39" t="s">
+        <v>332</v>
+      </c>
+      <c r="AB7" s="40" t="s">
+        <v>261</v>
+      </c>
+      <c r="AC7" s="40" t="s">
+        <v>262</v>
+      </c>
+      <c r="AD7" s="40" t="s">
+        <v>263</v>
+      </c>
+      <c r="AE7" s="39" t="s">
         <v>360</v>
       </c>
-      <c r="P7" s="51" t="s">
-        <v>233</v>
-      </c>
-      <c r="Q7" s="46" t="s">
+      <c r="AF7" s="39" t="s">
+        <v>359</v>
+      </c>
+      <c r="AG7" s="39" t="s">
+        <v>333</v>
+      </c>
+      <c r="AH7" s="39" t="s">
         <v>335</v>
       </c>
-      <c r="R7" s="46" t="s">
-        <v>244</v>
-      </c>
-      <c r="S7" s="46" t="s">
-        <v>234</v>
-      </c>
-      <c r="T7" s="48" t="s">
-        <v>235</v>
-      </c>
-      <c r="U7" s="48" t="s">
-        <v>359</v>
-      </c>
-      <c r="V7" s="48" t="s">
-        <v>242</v>
-      </c>
-      <c r="W7" s="48" t="s">
-        <v>243</v>
-      </c>
-      <c r="X7" s="48" t="s">
+      <c r="AI7" s="41" t="s">
         <v>336</v>
       </c>
-      <c r="Y7" s="48" t="s">
+      <c r="AJ7" s="34" t="s">
         <v>337</v>
       </c>
-      <c r="Z7" s="48" t="s">
-        <v>374</v>
-      </c>
-      <c r="AA7" s="51" t="s">
-        <v>338</v>
-      </c>
-      <c r="AB7" s="52" t="s">
-        <v>264</v>
-      </c>
-      <c r="AC7" s="52" t="s">
-        <v>265</v>
-      </c>
-      <c r="AD7" s="52" t="s">
-        <v>266</v>
-      </c>
-      <c r="AE7" s="51" t="s">
-        <v>367</v>
-      </c>
-      <c r="AF7" s="51" t="s">
-        <v>366</v>
-      </c>
-      <c r="AG7" s="51" t="s">
-        <v>339</v>
-      </c>
-      <c r="AH7" s="51" t="s">
-        <v>341</v>
-      </c>
-      <c r="AI7" s="53" t="s">
-        <v>342</v>
-      </c>
-      <c r="AJ7" s="46" t="s">
-        <v>343</v>
-      </c>
-    </row>
-    <row r="8" spans="1:36" s="30" customFormat="1" ht="66" thickBot="1">
-      <c r="A8" s="28" t="s">
-        <v>371</v>
+    </row>
+    <row r="8" spans="1:36" s="54" customFormat="1" ht="65">
+      <c r="A8" s="30" t="s">
+        <v>363</v>
       </c>
       <c r="B8" s="31"/>
       <c r="C8" s="32" t="s">
-        <v>365</v>
+        <v>358</v>
       </c>
       <c r="D8" s="32" t="s">
-        <v>365</v>
+        <v>358</v>
       </c>
       <c r="E8" s="33"/>
       <c r="F8" s="34" t="s">
-        <v>363</v>
+        <v>356</v>
       </c>
       <c r="G8" s="35"/>
       <c r="H8" s="36"/>
       <c r="I8" s="36"/>
       <c r="J8" s="37"/>
-      <c r="K8" s="28"/>
-      <c r="L8" s="28"/>
+      <c r="K8" s="30"/>
+      <c r="L8" s="30"/>
       <c r="M8" s="38"/>
       <c r="N8" s="38"/>
-      <c r="O8" s="29" t="s">
-        <v>361</v>
-      </c>
-      <c r="P8" s="29"/>
+      <c r="O8" s="39" t="s">
+        <v>354</v>
+      </c>
+      <c r="P8" s="39"/>
       <c r="Q8" s="34"/>
       <c r="R8" s="34"/>
       <c r="S8" s="34"/>
@@ -2567,86 +2623,130 @@
       <c r="V8" s="36"/>
       <c r="W8" s="36"/>
       <c r="X8" s="36" t="s">
-        <v>344</v>
+        <v>338</v>
       </c>
       <c r="Y8" s="36" t="s">
-        <v>344</v>
+        <v>338</v>
       </c>
       <c r="Z8" s="36" t="s">
-        <v>344</v>
+        <v>338</v>
       </c>
       <c r="AA8" s="31" t="s">
-        <v>344</v>
-      </c>
-      <c r="AB8" s="39"/>
-      <c r="AC8" s="39"/>
-      <c r="AD8" s="39"/>
-      <c r="AE8" s="29"/>
-      <c r="AF8" s="29"/>
-      <c r="AG8" s="29" t="s">
-        <v>340</v>
-      </c>
-      <c r="AH8" s="29" t="s">
-        <v>340</v>
-      </c>
-      <c r="AI8" s="40" t="s">
-        <v>340</v>
+        <v>338</v>
+      </c>
+      <c r="AB8" s="40"/>
+      <c r="AC8" s="40"/>
+      <c r="AD8" s="40"/>
+      <c r="AE8" s="39"/>
+      <c r="AF8" s="39"/>
+      <c r="AG8" s="39" t="s">
+        <v>334</v>
+      </c>
+      <c r="AH8" s="39" t="s">
+        <v>334</v>
+      </c>
+      <c r="AI8" s="41" t="s">
+        <v>334</v>
       </c>
       <c r="AJ8" s="34" t="s">
-        <v>344</v>
-      </c>
-    </row>
-    <row r="9" spans="1:36">
-      <c r="A9" s="14"/>
-      <c r="B9" s="15"/>
-      <c r="C9" s="23"/>
-      <c r="D9" s="23"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="2"/>
-      <c r="G9" s="7"/>
-      <c r="H9" s="17"/>
-      <c r="I9" s="17"/>
-      <c r="J9" s="18"/>
-      <c r="K9" s="14"/>
-      <c r="L9" s="14"/>
-      <c r="M9" s="19"/>
-      <c r="N9" s="19"/>
-      <c r="O9" s="16"/>
-      <c r="P9" s="16"/>
-      <c r="Q9" s="2"/>
-      <c r="R9" s="2"/>
-      <c r="S9" s="2"/>
-      <c r="T9" s="17"/>
-      <c r="U9" s="17"/>
-      <c r="V9" s="17"/>
-      <c r="W9" s="17"/>
-      <c r="X9" s="17"/>
-      <c r="Y9" s="17"/>
-      <c r="Z9" s="17"/>
-      <c r="AA9" s="17"/>
-      <c r="AB9" s="26"/>
-      <c r="AC9" s="26"/>
-      <c r="AD9" s="26"/>
-      <c r="AE9" s="16"/>
-      <c r="AF9" s="16"/>
-      <c r="AG9" s="16"/>
-      <c r="AH9" s="16"/>
-      <c r="AI9" s="20"/>
-      <c r="AJ9" s="2"/>
+        <v>338</v>
+      </c>
+    </row>
+    <row r="9" spans="1:36" s="28" customFormat="1" ht="16" customHeight="1" thickBot="1">
+      <c r="A9" s="42" t="s">
+        <v>367</v>
+      </c>
+      <c r="B9" s="43"/>
+      <c r="C9" s="44"/>
+      <c r="D9" s="44"/>
+      <c r="E9" s="45" t="s">
+        <v>369</v>
+      </c>
+      <c r="F9" s="46" t="s">
+        <v>368</v>
+      </c>
+      <c r="G9" s="47"/>
+      <c r="H9" s="48"/>
+      <c r="I9" s="48"/>
+      <c r="J9" s="49"/>
+      <c r="K9" s="42"/>
+      <c r="L9" s="42"/>
+      <c r="M9" s="50"/>
+      <c r="N9" s="50"/>
+      <c r="O9" s="51"/>
+      <c r="P9" s="51"/>
+      <c r="Q9" s="46"/>
+      <c r="R9" s="46"/>
+      <c r="S9" s="46"/>
+      <c r="T9" s="48"/>
+      <c r="U9" s="48"/>
+      <c r="V9" s="48"/>
+      <c r="W9" s="48"/>
+      <c r="X9" s="48"/>
+      <c r="Y9" s="48"/>
+      <c r="Z9" s="48"/>
+      <c r="AA9" s="43"/>
+      <c r="AB9" s="52"/>
+      <c r="AC9" s="52"/>
+      <c r="AD9" s="52"/>
+      <c r="AE9" s="51"/>
+      <c r="AF9" s="51"/>
+      <c r="AG9" s="51"/>
+      <c r="AH9" s="51"/>
+      <c r="AI9" s="53"/>
+      <c r="AJ9" s="46"/>
+    </row>
+    <row r="10" spans="1:36">
+      <c r="A10" s="14"/>
+      <c r="B10" s="15"/>
+      <c r="C10" s="23"/>
+      <c r="D10" s="23"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="7"/>
+      <c r="H10" s="17"/>
+      <c r="I10" s="17"/>
+      <c r="J10" s="18"/>
+      <c r="K10" s="14"/>
+      <c r="L10" s="14"/>
+      <c r="M10" s="19"/>
+      <c r="N10" s="19"/>
+      <c r="O10" s="16"/>
+      <c r="P10" s="16"/>
+      <c r="Q10" s="2"/>
+      <c r="R10" s="2"/>
+      <c r="S10" s="2"/>
+      <c r="T10" s="17"/>
+      <c r="U10" s="17"/>
+      <c r="V10" s="17"/>
+      <c r="W10" s="17"/>
+      <c r="X10" s="17"/>
+      <c r="Y10" s="17"/>
+      <c r="Z10" s="17"/>
+      <c r="AA10" s="17"/>
+      <c r="AB10" s="26"/>
+      <c r="AC10" s="26"/>
+      <c r="AD10" s="26"/>
+      <c r="AE10" s="16"/>
+      <c r="AF10" s="16"/>
+      <c r="AG10" s="16"/>
+      <c r="AH10" s="16"/>
+      <c r="AI10" s="20"/>
+      <c r="AJ10" s="2"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <dataValidations count="4">
-    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="T9:T1048576">
+    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="T10:T1048576">
       <formula1>"cc-by,cc-by-nc,cc-by-sa,cc-by-nc-sa,public domain,not applicable"</formula1>
     </dataValidation>
-    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E9:E1048576">
+    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E10:E1048576">
       <formula1>DataTypeTerms</formula1>
     </dataValidation>
-    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F9:F1048576">
+    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F10:F1048576">
       <formula1>DataSubtypeTerms</formula1>
     </dataValidation>
-    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H9:H1048576">
+    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H10:H1048576">
       <formula1>SubjectTerms</formula1>
     </dataValidation>
   </dataValidations>
@@ -2662,11 +2762,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O9"/>
+  <dimension ref="A1:O10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="8" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+      <pane ySplit="9" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="O2" sqref="O2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
@@ -2684,43 +2784,43 @@
   <sheetData>
     <row r="1" spans="1:15" s="21" customFormat="1" ht="24" customHeight="1" thickBot="1">
       <c r="A1" s="21" t="s">
+        <v>133</v>
+      </c>
+      <c r="B1" s="21" t="s">
         <v>135</v>
       </c>
-      <c r="B1" s="21" t="s">
-        <v>137</v>
-      </c>
       <c r="C1" s="21" t="s">
+        <v>182</v>
+      </c>
+      <c r="D1" s="21" t="s">
+        <v>183</v>
+      </c>
+      <c r="E1" s="21" t="s">
+        <v>184</v>
+      </c>
+      <c r="F1" s="21" t="s">
         <v>185</v>
       </c>
-      <c r="D1" s="21" t="s">
+      <c r="G1" s="21" t="s">
         <v>186</v>
       </c>
-      <c r="E1" s="21" t="s">
+      <c r="H1" s="21" t="s">
         <v>187</v>
       </c>
-      <c r="F1" s="21" t="s">
+      <c r="I1" s="21" t="s">
         <v>188</v>
       </c>
-      <c r="G1" s="21" t="s">
+      <c r="J1" s="21" t="s">
         <v>189</v>
       </c>
-      <c r="H1" s="21" t="s">
+      <c r="K1" s="21" t="s">
+        <v>192</v>
+      </c>
+      <c r="L1" s="21" t="s">
+        <v>195</v>
+      </c>
+      <c r="M1" s="21" t="s">
         <v>190</v>
-      </c>
-      <c r="I1" s="21" t="s">
-        <v>191</v>
-      </c>
-      <c r="J1" s="21" t="s">
-        <v>192</v>
-      </c>
-      <c r="K1" s="21" t="s">
-        <v>195</v>
-      </c>
-      <c r="L1" s="21" t="s">
-        <v>198</v>
-      </c>
-      <c r="M1" s="21" t="s">
-        <v>193</v>
       </c>
       <c r="N1" s="21" t="s">
         <v>44</v>
@@ -2731,124 +2831,128 @@
     </row>
     <row r="2" spans="1:15">
       <c r="A2" s="14" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="C2" t="s">
         <v>43</v>
       </c>
       <c r="D2" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2" t="s">
+        <v>53</v>
+      </c>
+      <c r="F2" t="s">
         <v>55</v>
       </c>
-      <c r="E2" t="s">
-        <v>54</v>
-      </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>56</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>57</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>58</v>
       </c>
-      <c r="I2" t="s">
-        <v>59</v>
-      </c>
       <c r="J2" t="s">
+        <v>60</v>
+      </c>
+      <c r="K2" t="s">
+        <v>115</v>
+      </c>
+      <c r="L2" t="s">
+        <v>196</v>
+      </c>
+      <c r="M2" t="s">
         <v>62</v>
       </c>
-      <c r="K2" t="s">
-        <v>117</v>
-      </c>
-      <c r="L2" t="s">
-        <v>199</v>
-      </c>
-      <c r="M2" t="s">
-        <v>64</v>
-      </c>
       <c r="N2" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="O2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="3" spans="1:15">
       <c r="A3" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="4" spans="1:15">
       <c r="C4" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="O4" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15" s="41" customFormat="1" ht="159" customHeight="1">
-      <c r="A7" s="42" t="s">
-        <v>222</v>
-      </c>
-      <c r="B7" s="51" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" s="29" customFormat="1" ht="159" customHeight="1">
+      <c r="A7" s="30" t="s">
+        <v>219</v>
+      </c>
+      <c r="B7" s="39" t="s">
+        <v>242</v>
+      </c>
+      <c r="C7" s="29" t="s">
+        <v>243</v>
+      </c>
+      <c r="D7" s="29" t="s">
+        <v>244</v>
+      </c>
+      <c r="E7" s="29" t="s">
         <v>245</v>
       </c>
-      <c r="C7" s="41" t="s">
+      <c r="F7" s="29" t="s">
         <v>246</v>
       </c>
-      <c r="D7" s="41" t="s">
+      <c r="G7" s="29" t="s">
         <v>247</v>
       </c>
-      <c r="E7" s="41" t="s">
+      <c r="H7" s="29" t="s">
         <v>248</v>
       </c>
-      <c r="F7" s="41" t="s">
+      <c r="I7" s="29" t="s">
         <v>249</v>
       </c>
-      <c r="G7" s="41" t="s">
+      <c r="J7" s="29" t="s">
         <v>250</v>
       </c>
-      <c r="H7" s="41" t="s">
+      <c r="K7" s="29" t="s">
         <v>251</v>
       </c>
-      <c r="I7" s="41" t="s">
+      <c r="L7" s="29" t="s">
         <v>252</v>
       </c>
-      <c r="J7" s="41" t="s">
+      <c r="M7" s="29" t="s">
         <v>253</v>
       </c>
-      <c r="K7" s="41" t="s">
+      <c r="N7" s="29" t="s">
         <v>254</v>
       </c>
-      <c r="L7" s="41" t="s">
-        <v>255</v>
-      </c>
-      <c r="M7" s="41" t="s">
-        <v>256</v>
-      </c>
-      <c r="N7" s="41" t="s">
-        <v>257</v>
-      </c>
-      <c r="O7" s="41" t="s">
-        <v>343</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15" s="30" customFormat="1" ht="40" thickBot="1">
-      <c r="A8" s="28"/>
-      <c r="B8" s="29"/>
-      <c r="O8" s="30" t="s">
-        <v>344</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15">
-      <c r="A9" s="14"/>
-      <c r="B9" s="16"/>
+      <c r="O7" s="29" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" s="54" customFormat="1" ht="39">
+      <c r="A8" s="30"/>
+      <c r="B8" s="39"/>
+      <c r="O8" s="54" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" s="28" customFormat="1" ht="14" thickBot="1">
+      <c r="A9" s="42"/>
+      <c r="B9" s="51"/>
+    </row>
+    <row r="10" spans="1:15">
+      <c r="A10" s="14"/>
+      <c r="B10" s="16"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -2861,13 +2965,13 @@
           <x14:formula1>
             <xm:f>'controlled terms'!$F$2:$F$29</xm:f>
           </x14:formula1>
-          <xm:sqref>J9:J1048576</xm:sqref>
+          <xm:sqref>J10:J1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>'controlled terms'!$G$2:$G$9</xm:f>
           </x14:formula1>
-          <xm:sqref>L9:L1048576</xm:sqref>
+          <xm:sqref>L10:L1048576</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -2880,10 +2984,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H8"/>
+  <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="8" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="9" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
@@ -2901,106 +3005,110 @@
   <sheetData>
     <row r="1" spans="1:8" s="21" customFormat="1" ht="24" customHeight="1" thickBot="1">
       <c r="A1" s="21" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="B1" s="21" t="s">
+        <v>64</v>
+      </c>
+      <c r="C1" s="21" t="s">
         <v>66</v>
       </c>
-      <c r="C1" s="21" t="s">
+      <c r="D1" s="21" t="s">
+        <v>193</v>
+      </c>
+      <c r="E1" s="21" t="s">
         <v>68</v>
       </c>
-      <c r="D1" s="21" t="s">
-        <v>196</v>
-      </c>
-      <c r="E1" s="21" t="s">
-        <v>70</v>
-      </c>
       <c r="F1" s="21" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="G1" s="21" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="H1" s="21" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
     </row>
     <row r="2" spans="1:8">
       <c r="A2" s="14" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="B2" s="16" t="s">
+        <v>65</v>
+      </c>
+      <c r="C2" t="s">
         <v>67</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
+        <v>118</v>
+      </c>
+      <c r="E2" t="s">
         <v>69</v>
       </c>
-      <c r="D2" t="s">
-        <v>120</v>
-      </c>
-      <c r="E2" t="s">
-        <v>71</v>
-      </c>
       <c r="F2" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="G2" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="H2" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="3" spans="1:8">
       <c r="A3" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="4" spans="1:8">
       <c r="A4" s="6" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
     </row>
     <row r="6" spans="1:8">
       <c r="D6" t="s">
-        <v>368</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" s="41" customFormat="1" ht="143">
-      <c r="A7" s="42" t="s">
-        <v>222</v>
-      </c>
-      <c r="B7" s="51" t="s">
-        <v>224</v>
-      </c>
-      <c r="C7" s="41" t="s">
-        <v>262</v>
-      </c>
-      <c r="D7" s="41" t="s">
-        <v>263</v>
-      </c>
-      <c r="E7" s="41" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" s="29" customFormat="1" ht="143">
+      <c r="A7" s="30" t="s">
+        <v>219</v>
+      </c>
+      <c r="B7" s="39" t="s">
+        <v>221</v>
+      </c>
+      <c r="C7" s="29" t="s">
+        <v>259</v>
+      </c>
+      <c r="D7" s="29" t="s">
         <v>260</v>
       </c>
-      <c r="F7" s="41" t="s">
-        <v>261</v>
-      </c>
-      <c r="G7" s="41" t="s">
+      <c r="E7" s="29" t="s">
+        <v>257</v>
+      </c>
+      <c r="F7" s="29" t="s">
         <v>258</v>
       </c>
-      <c r="H7" s="41" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" s="30" customFormat="1" ht="14" thickBot="1">
-      <c r="A8" s="28"/>
-      <c r="B8" s="29"/>
+      <c r="G7" s="29" t="s">
+        <v>255</v>
+      </c>
+      <c r="H7" s="29" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" s="54" customFormat="1">
+      <c r="A8" s="30"/>
+      <c r="B8" s="39"/>
+    </row>
+    <row r="9" spans="1:8" s="28" customFormat="1" ht="14" thickBot="1">
+      <c r="A9" s="42"/>
+      <c r="B9" s="51"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -3016,10 +3124,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R8"/>
+  <dimension ref="A1:R9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="8" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="9" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
@@ -3045,93 +3153,93 @@
   <sheetData>
     <row r="1" spans="1:18" s="21" customFormat="1" ht="24" customHeight="1" thickBot="1">
       <c r="A1" s="21" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="B1" s="21" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="C1" s="21" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="D1" s="21" t="s">
-        <v>293</v>
+        <v>288</v>
       </c>
       <c r="E1" s="21" t="s">
-        <v>294</v>
+        <v>289</v>
       </c>
       <c r="F1" s="21" t="s">
+        <v>200</v>
+      </c>
+      <c r="G1" s="21" t="s">
+        <v>201</v>
+      </c>
+      <c r="H1" s="21" t="s">
+        <v>202</v>
+      </c>
+      <c r="I1" s="21" t="s">
         <v>203</v>
       </c>
-      <c r="G1" s="21" t="s">
+      <c r="J1" s="21" t="s">
         <v>204</v>
       </c>
-      <c r="H1" s="21" t="s">
+      <c r="K1" s="21" t="s">
         <v>205</v>
       </c>
-      <c r="I1" s="21" t="s">
+      <c r="L1" s="21" t="s">
         <v>206</v>
       </c>
-      <c r="J1" s="21" t="s">
+      <c r="M1" s="21" t="s">
+        <v>233</v>
+      </c>
+      <c r="N1" s="21" t="s">
+        <v>234</v>
+      </c>
+      <c r="O1" s="21" t="s">
         <v>207</v>
       </c>
-      <c r="K1" s="21" t="s">
+      <c r="P1" s="21" t="s">
         <v>208</v>
       </c>
-      <c r="L1" s="21" t="s">
+      <c r="Q1" s="21" t="s">
         <v>209</v>
       </c>
-      <c r="M1" s="21" t="s">
-        <v>236</v>
-      </c>
-      <c r="N1" s="21" t="s">
-        <v>237</v>
-      </c>
-      <c r="O1" s="21" t="s">
-        <v>210</v>
-      </c>
-      <c r="P1" s="21" t="s">
-        <v>211</v>
-      </c>
-      <c r="Q1" s="21" t="s">
-        <v>212</v>
-      </c>
       <c r="R1" s="21" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
     </row>
     <row r="2" spans="1:18" ht="14" thickTop="1">
       <c r="A2" s="14" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="B2" t="s">
-        <v>292</v>
+        <v>375</v>
       </c>
       <c r="C2" s="16" t="s">
-        <v>151</v>
+        <v>373</v>
       </c>
       <c r="D2" t="s">
-        <v>295</v>
+        <v>374</v>
       </c>
       <c r="E2" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="F2" t="s">
+        <v>145</v>
+      </c>
+      <c r="G2" t="s">
+        <v>144</v>
+      </c>
+      <c r="H2" t="s">
+        <v>146</v>
+      </c>
+      <c r="I2" t="s">
         <v>147</v>
       </c>
-      <c r="G2" t="s">
-        <v>146</v>
-      </c>
-      <c r="H2" t="s">
+      <c r="J2" t="s">
         <v>148</v>
       </c>
-      <c r="I2" t="s">
-        <v>149</v>
-      </c>
-      <c r="J2" t="s">
-        <v>150</v>
-      </c>
       <c r="K2" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="L2" t="s">
         <v>41</v>
@@ -3140,93 +3248,97 @@
         <v>42</v>
       </c>
       <c r="N2" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="O2" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="P2" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="Q2" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="R2" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
     </row>
     <row r="3" spans="1:18">
       <c r="A3" s="6" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
     </row>
     <row r="6" spans="1:18">
       <c r="O6" t="s">
-        <v>368</v>
-      </c>
-    </row>
-    <row r="7" spans="1:18" s="41" customFormat="1" ht="140" customHeight="1">
-      <c r="A7" s="42" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" s="29" customFormat="1" ht="140" customHeight="1">
+      <c r="A7" s="30" t="s">
+        <v>264</v>
+      </c>
+      <c r="B7" s="29" t="s">
+        <v>370</v>
+      </c>
+      <c r="C7" s="39" t="s">
+        <v>272</v>
+      </c>
+      <c r="D7" s="29" t="s">
+        <v>364</v>
+      </c>
+      <c r="E7" s="29" t="s">
+        <v>365</v>
+      </c>
+      <c r="F7" s="29" t="s">
+        <v>265</v>
+      </c>
+      <c r="G7" s="29" t="s">
+        <v>266</v>
+      </c>
+      <c r="H7" s="29" t="s">
         <v>267</v>
       </c>
-      <c r="B7" s="41" t="s">
-        <v>291</v>
-      </c>
-      <c r="C7" s="51" t="s">
+      <c r="I7" s="29" t="s">
+        <v>268</v>
+      </c>
+      <c r="J7" s="29" t="s">
+        <v>269</v>
+      </c>
+      <c r="K7" s="29" t="s">
+        <v>277</v>
+      </c>
+      <c r="L7" s="29" t="s">
+        <v>286</v>
+      </c>
+      <c r="M7" s="29" t="s">
+        <v>270</v>
+      </c>
+      <c r="N7" s="29" t="s">
+        <v>353</v>
+      </c>
+      <c r="O7" s="29" t="s">
+        <v>276</v>
+      </c>
+      <c r="P7" s="29" t="s">
         <v>275</v>
       </c>
-      <c r="D7" s="41" t="s">
-        <v>372</v>
-      </c>
-      <c r="E7" s="41" t="s">
-        <v>373</v>
-      </c>
-      <c r="F7" s="41" t="s">
-        <v>268</v>
-      </c>
-      <c r="G7" s="41" t="s">
-        <v>269</v>
-      </c>
-      <c r="H7" s="41" t="s">
-        <v>270</v>
-      </c>
-      <c r="I7" s="41" t="s">
-        <v>271</v>
-      </c>
-      <c r="J7" s="41" t="s">
-        <v>272</v>
-      </c>
-      <c r="K7" s="41" t="s">
-        <v>280</v>
-      </c>
-      <c r="L7" s="41" t="s">
-        <v>289</v>
-      </c>
-      <c r="M7" s="41" t="s">
+      <c r="Q7" s="29" t="s">
+        <v>274</v>
+      </c>
+      <c r="R7" s="29" t="s">
         <v>273</v>
       </c>
-      <c r="N7" s="41" t="s">
-        <v>360</v>
-      </c>
-      <c r="O7" s="41" t="s">
-        <v>279</v>
-      </c>
-      <c r="P7" s="41" t="s">
-        <v>278</v>
-      </c>
-      <c r="Q7" s="41" t="s">
-        <v>277</v>
-      </c>
-      <c r="R7" s="41" t="s">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="8" spans="1:18" s="30" customFormat="1" ht="27" thickBot="1">
-      <c r="A8" s="28"/>
-      <c r="C8" s="29"/>
-      <c r="N8" s="30" t="s">
-        <v>361</v>
-      </c>
+    </row>
+    <row r="8" spans="1:18" s="54" customFormat="1" ht="26">
+      <c r="A8" s="30"/>
+      <c r="C8" s="39"/>
+      <c r="N8" s="54" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" s="28" customFormat="1" ht="14" thickBot="1">
+      <c r="A9" s="42"/>
+      <c r="C9" s="51"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -3242,10 +3354,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L8"/>
+  <dimension ref="A1:L9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="8" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="9" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
@@ -3302,93 +3414,97 @@
     </row>
     <row r="2" spans="1:12" ht="14" thickTop="1">
       <c r="A2" s="14" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="B2" s="16" t="s">
+        <v>278</v>
+      </c>
+      <c r="C2" t="s">
         <v>281</v>
       </c>
-      <c r="C2" t="s">
-        <v>284</v>
-      </c>
       <c r="D2" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="E2" t="s">
-        <v>370</v>
+        <v>376</v>
       </c>
       <c r="F2" t="s">
-        <v>345</v>
+        <v>339</v>
       </c>
       <c r="G2" t="s">
-        <v>346</v>
+        <v>340</v>
       </c>
       <c r="H2" t="s">
-        <v>347</v>
+        <v>341</v>
       </c>
       <c r="I2" t="s">
-        <v>348</v>
+        <v>342</v>
       </c>
       <c r="J2" t="s">
-        <v>354</v>
+        <v>377</v>
       </c>
       <c r="K2" t="s">
-        <v>350</v>
+        <v>344</v>
       </c>
       <c r="L2" t="s">
-        <v>349</v>
+        <v>343</v>
       </c>
     </row>
     <row r="3" spans="1:12">
       <c r="A3" s="6" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" s="41" customFormat="1" ht="91">
-      <c r="A7" s="42" t="s">
-        <v>267</v>
-      </c>
-      <c r="B7" s="51" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" s="29" customFormat="1" ht="91">
+      <c r="A7" s="30" t="s">
+        <v>264</v>
+      </c>
+      <c r="B7" s="39" t="s">
+        <v>279</v>
+      </c>
+      <c r="C7" s="29" t="s">
+        <v>280</v>
+      </c>
+      <c r="D7" s="29" t="s">
         <v>282</v>
       </c>
-      <c r="C7" s="41" t="s">
-        <v>283</v>
-      </c>
-      <c r="D7" s="41" t="s">
-        <v>285</v>
-      </c>
-      <c r="E7" s="41" t="s">
-        <v>358</v>
-      </c>
-      <c r="F7" s="41" t="s">
-        <v>357</v>
-      </c>
-      <c r="G7" s="41" t="s">
-        <v>356</v>
-      </c>
-      <c r="H7" s="41" t="s">
-        <v>355</v>
-      </c>
-      <c r="I7" s="41" t="s">
-        <v>352</v>
-      </c>
-      <c r="J7" s="41" t="s">
-        <v>353</v>
-      </c>
-      <c r="K7" s="41" t="s">
+      <c r="E7" s="29" t="s">
         <v>351</v>
       </c>
-      <c r="L7" s="41" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" s="30" customFormat="1" ht="14" thickBot="1">
-      <c r="A8" s="28"/>
-      <c r="B8" s="29"/>
+      <c r="F7" s="29" t="s">
+        <v>350</v>
+      </c>
+      <c r="G7" s="29" t="s">
+        <v>349</v>
+      </c>
+      <c r="H7" s="29" t="s">
+        <v>348</v>
+      </c>
+      <c r="I7" s="29" t="s">
+        <v>346</v>
+      </c>
+      <c r="J7" s="29" t="s">
+        <v>347</v>
+      </c>
+      <c r="K7" s="29" t="s">
+        <v>345</v>
+      </c>
+      <c r="L7" s="29" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" s="54" customFormat="1">
+      <c r="A8" s="30"/>
+      <c r="B8" s="39"/>
+    </row>
+    <row r="9" spans="1:12" s="28" customFormat="1" ht="14" thickBot="1">
+      <c r="A9" s="42"/>
+      <c r="B9" s="51"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E9:E1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E10:E1048576">
       <formula1>AgentRoleTerms</formula1>
     </dataValidation>
   </dataValidations>
@@ -3425,22 +3541,22 @@
         <v>18</v>
       </c>
       <c r="B1" s="21" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C1" s="21" t="s">
         <v>19</v>
       </c>
       <c r="D1" s="21" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="E1" s="21" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="F1" s="21" t="s">
-        <v>297</v>
+        <v>291</v>
       </c>
       <c r="G1" s="21" t="s">
-        <v>334</v>
+        <v>328</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -3454,16 +3570,16 @@
         <v>24</v>
       </c>
       <c r="D2" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="E2" t="s">
         <v>1</v>
       </c>
       <c r="F2" t="s">
-        <v>298</v>
+        <v>292</v>
       </c>
       <c r="G2" t="s">
-        <v>326</v>
+        <v>320</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -3474,16 +3590,16 @@
         <v>21</v>
       </c>
       <c r="D3" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E3" t="s">
         <v>2</v>
       </c>
       <c r="F3" t="s">
-        <v>299</v>
+        <v>293</v>
       </c>
       <c r="G3" t="s">
-        <v>327</v>
+        <v>321</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -3494,16 +3610,16 @@
         <v>22</v>
       </c>
       <c r="D4" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="E4" t="s">
         <v>4</v>
       </c>
       <c r="F4" t="s">
-        <v>300</v>
+        <v>294</v>
       </c>
       <c r="G4" t="s">
-        <v>328</v>
+        <v>322</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -3514,33 +3630,33 @@
         <v>23</v>
       </c>
       <c r="D5" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="E5" t="s">
         <v>5</v>
       </c>
       <c r="F5" t="s">
-        <v>301</v>
+        <v>295</v>
       </c>
       <c r="G5" t="s">
-        <v>329</v>
+        <v>323</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="A6" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="D6" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="E6" t="s">
         <v>0</v>
       </c>
       <c r="F6" t="s">
-        <v>302</v>
+        <v>296</v>
       </c>
       <c r="G6" t="s">
-        <v>330</v>
+        <v>324</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -3548,16 +3664,16 @@
         <v>29</v>
       </c>
       <c r="D7" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="E7" t="s">
         <v>3</v>
       </c>
       <c r="F7" t="s">
-        <v>303</v>
+        <v>297</v>
       </c>
       <c r="G7" t="s">
-        <v>331</v>
+        <v>325</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -3565,13 +3681,13 @@
         <v>30</v>
       </c>
       <c r="D8" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="F8" t="s">
-        <v>304</v>
+        <v>298</v>
       </c>
       <c r="G8" t="s">
-        <v>332</v>
+        <v>326</v>
       </c>
     </row>
     <row r="9" spans="1:7">
@@ -3579,13 +3695,13 @@
         <v>31</v>
       </c>
       <c r="D9" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="F9" t="s">
-        <v>305</v>
+        <v>299</v>
       </c>
       <c r="G9" t="s">
-        <v>333</v>
+        <v>327</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -3593,10 +3709,10 @@
         <v>32</v>
       </c>
       <c r="D10" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="F10" t="s">
-        <v>306</v>
+        <v>300</v>
       </c>
     </row>
     <row r="11" spans="1:7">
@@ -3604,10 +3720,10 @@
         <v>33</v>
       </c>
       <c r="D11" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="F11" t="s">
-        <v>307</v>
+        <v>301</v>
       </c>
     </row>
     <row r="12" spans="1:7">
@@ -3615,10 +3731,10 @@
         <v>34</v>
       </c>
       <c r="D12" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="F12" t="s">
-        <v>308</v>
+        <v>302</v>
       </c>
     </row>
     <row r="13" spans="1:7">
@@ -3626,10 +3742,10 @@
         <v>35</v>
       </c>
       <c r="D13" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="F13" t="s">
-        <v>309</v>
+        <v>303</v>
       </c>
     </row>
     <row r="14" spans="1:7">
@@ -3637,10 +3753,10 @@
         <v>36</v>
       </c>
       <c r="D14" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="F14" t="s">
-        <v>310</v>
+        <v>304</v>
       </c>
     </row>
     <row r="15" spans="1:7">
@@ -3648,172 +3764,172 @@
         <v>37</v>
       </c>
       <c r="D15" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="F15" t="s">
-        <v>311</v>
+        <v>305</v>
       </c>
     </row>
     <row r="16" spans="1:7">
       <c r="D16" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="F16" t="s">
-        <v>312</v>
+        <v>306</v>
       </c>
     </row>
     <row r="17" spans="4:6">
       <c r="D17" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="F17" t="s">
-        <v>313</v>
+        <v>307</v>
       </c>
     </row>
     <row r="18" spans="4:6">
       <c r="D18" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="F18" t="s">
-        <v>314</v>
+        <v>308</v>
       </c>
     </row>
     <row r="19" spans="4:6">
       <c r="D19" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="F19" t="s">
-        <v>315</v>
+        <v>309</v>
       </c>
     </row>
     <row r="20" spans="4:6">
       <c r="D20" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="F20" t="s">
-        <v>316</v>
+        <v>310</v>
       </c>
     </row>
     <row r="21" spans="4:6">
       <c r="D21" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="F21" t="s">
-        <v>317</v>
+        <v>311</v>
       </c>
     </row>
     <row r="22" spans="4:6">
       <c r="D22" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="F22" t="s">
-        <v>318</v>
+        <v>312</v>
       </c>
     </row>
     <row r="23" spans="4:6">
       <c r="D23" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F23" t="s">
-        <v>319</v>
+        <v>313</v>
       </c>
     </row>
     <row r="24" spans="4:6">
       <c r="D24" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="F24" t="s">
-        <v>320</v>
+        <v>314</v>
       </c>
     </row>
     <row r="25" spans="4:6">
       <c r="D25" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="F25" t="s">
-        <v>321</v>
+        <v>315</v>
       </c>
     </row>
     <row r="26" spans="4:6">
       <c r="D26" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="F26" t="s">
-        <v>322</v>
+        <v>316</v>
       </c>
     </row>
     <row r="27" spans="4:6">
       <c r="D27" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="F27" t="s">
-        <v>323</v>
+        <v>317</v>
       </c>
     </row>
     <row r="28" spans="4:6">
       <c r="D28" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="F28" t="s">
-        <v>324</v>
+        <v>318</v>
       </c>
     </row>
     <row r="29" spans="4:6">
       <c r="D29" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="F29" t="s">
-        <v>325</v>
+        <v>319</v>
       </c>
     </row>
     <row r="30" spans="4:6">
       <c r="D30" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="31" spans="4:6">
       <c r="D31" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="32" spans="4:6">
       <c r="D32" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="33" spans="4:4">
       <c r="D33" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="34" spans="4:4">
       <c r="D34" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="35" spans="4:4">
       <c r="D35" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="36" spans="4:4">
       <c r="D36" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="37" spans="4:4">
       <c r="D37" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="38" spans="4:4">
       <c r="D38" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="39" spans="4:4">
       <c r="D39" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
   </sheetData>

</xml_diff>